<commit_message>
Added weather data and descriptions
</commit_message>
<xml_diff>
--- a/Energy_Data_Dictionary.xlsx
+++ b/Energy_Data_Dictionary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Sofia/Desktop/Education/UNIPD/Fall 2023/Business Economic and Financial Data/project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matti\Documents\GitHub\business_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EC7F93B-46DA-9D4B-84C4-8DC563478B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE2AC30-9A70-4B1D-8B7C-875B4CEFFC9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="500" windowWidth="27480" windowHeight="16940" xr2:uid="{0CF4C3A6-E06D-554F-B889-D0605F8E8A88}"/>
+    <workbookView xWindow="10440" yWindow="840" windowWidth="21640" windowHeight="11690" xr2:uid="{0CF4C3A6-E06D-554F-B889-D0605F8E8A88}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="105">
   <si>
     <t xml:space="preserve">DATE                                            </t>
   </si>
@@ -296,6 +296,60 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>tavg</t>
+  </si>
+  <si>
+    <t>tmin</t>
+  </si>
+  <si>
+    <t>tmax</t>
+  </si>
+  <si>
+    <t>prcp</t>
+  </si>
+  <si>
+    <t>wspd</t>
+  </si>
+  <si>
+    <t>Float64</t>
+  </si>
+  <si>
+    <t>pres</t>
+  </si>
+  <si>
+    <t>°C</t>
+  </si>
+  <si>
+    <t>mm</t>
+  </si>
+  <si>
+    <t>km/h</t>
+  </si>
+  <si>
+    <t>hPa</t>
+  </si>
+  <si>
+    <t>Weather</t>
+  </si>
+  <si>
+    <t>Average air temperature</t>
+  </si>
+  <si>
+    <t>Minimum air temperature</t>
+  </si>
+  <si>
+    <t>Maximum air temperature</t>
+  </si>
+  <si>
+    <t>Precipitation total</t>
+  </si>
+  <si>
+    <t>Wind speed</t>
+  </si>
+  <si>
+    <t>Average sea-level air pressure</t>
   </si>
 </sst>
 </file>
@@ -647,13 +701,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EABD4BD-3672-7346-AAAF-B604F2036DFC}">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="41" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.5" bestFit="1" customWidth="1"/>
@@ -662,7 +716,7 @@
     <col min="6" max="6" width="64.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>33</v>
       </c>
@@ -682,7 +736,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -702,7 +756,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -722,7 +776,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -742,7 +796,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -762,7 +816,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -782,7 +836,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -802,7 +856,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -822,7 +876,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -842,7 +896,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -862,7 +916,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -882,7 +936,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -902,7 +956,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -922,7 +976,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -942,7 +996,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -962,7 +1016,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -982,7 +1036,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1002,7 +1056,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1022,7 +1076,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1042,7 +1096,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1062,7 +1116,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1082,7 +1136,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1102,7 +1156,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1122,7 +1176,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1142,7 +1196,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1162,7 +1216,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1182,7 +1236,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1202,7 +1256,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1222,7 +1276,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1242,7 +1296,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1262,7 +1316,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1282,7 +1336,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1302,7 +1356,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1322,7 +1376,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1340,6 +1394,126 @@
       </c>
       <c r="F34" t="s">
         <v>66</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>87</v>
+      </c>
+      <c r="B35">
+        <v>34</v>
+      </c>
+      <c r="C35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" t="s">
+        <v>94</v>
+      </c>
+      <c r="E35" t="s">
+        <v>98</v>
+      </c>
+      <c r="F35" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>88</v>
+      </c>
+      <c r="B36">
+        <v>35</v>
+      </c>
+      <c r="C36" t="s">
+        <v>92</v>
+      </c>
+      <c r="D36" t="s">
+        <v>94</v>
+      </c>
+      <c r="E36" t="s">
+        <v>98</v>
+      </c>
+      <c r="F36" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>89</v>
+      </c>
+      <c r="B37">
+        <v>36</v>
+      </c>
+      <c r="C37" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" t="s">
+        <v>94</v>
+      </c>
+      <c r="E37" t="s">
+        <v>98</v>
+      </c>
+      <c r="F37" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B38">
+        <v>37</v>
+      </c>
+      <c r="C38" t="s">
+        <v>92</v>
+      </c>
+      <c r="D38" t="s">
+        <v>95</v>
+      </c>
+      <c r="E38" t="s">
+        <v>98</v>
+      </c>
+      <c r="F38" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>91</v>
+      </c>
+      <c r="B39">
+        <v>38</v>
+      </c>
+      <c r="C39" t="s">
+        <v>92</v>
+      </c>
+      <c r="D39" t="s">
+        <v>96</v>
+      </c>
+      <c r="E39" t="s">
+        <v>98</v>
+      </c>
+      <c r="F39" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>93</v>
+      </c>
+      <c r="B40">
+        <v>39</v>
+      </c>
+      <c r="C40" t="s">
+        <v>92</v>
+      </c>
+      <c r="D40" t="s">
+        <v>97</v>
+      </c>
+      <c r="E40" t="s">
+        <v>98</v>
+      </c>
+      <c r="F40" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>